<commit_message>
First set of model updates for PL
</commit_message>
<xml_diff>
--- a/input/align_educLevel.xlsx
+++ b/input/align_educLevel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPaths_HU\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFFB082-9815-4486-8A50-726EE85492DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F2D5C3-0E13-4567-B019-D79EDF01BD18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="5" xr2:uid="{8B3B1A3D-54CF-4240-A44B-2FEE87419FDF}"/>
   </bookViews>
@@ -17,8 +17,8 @@
     <sheet name="UK_Low" sheetId="2" r:id="rId2"/>
     <sheet name="IT_High" sheetId="3" r:id="rId3"/>
     <sheet name="IT_Low" sheetId="4" r:id="rId4"/>
-    <sheet name="HU_High" sheetId="5" r:id="rId5"/>
-    <sheet name="HU_Low" sheetId="6" r:id="rId6"/>
+    <sheet name="PL_High" sheetId="5" r:id="rId5"/>
+    <sheet name="PL_Low" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>